<commit_message>
Updated models: Rice perc and wheat perc as moving average of past 3 years with results on model summary.xlsx and code in section4_oldcode.R
</commit_message>
<xml_diff>
--- a/Model Summary.xlsx
+++ b/Model Summary.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Model</t>
   </si>
@@ -24,34 +24,28 @@
     <t>R squared</t>
   </si>
   <si>
-    <t>Rice Alt ~ Pop + rice_perc + wheat_perc ( as individual)</t>
-  </si>
-  <si>
-    <t>Rice alt ~ Pop + rice_perc + wheat_perc ( as average )</t>
-  </si>
-  <si>
-    <t>Wheat alt ~ Pop + rice_perc + wheat_perc ( as average )</t>
-  </si>
-  <si>
-    <t>Wheat alt ~ Pop + rice_perc + wheat_perc ( as individual )</t>
-  </si>
-  <si>
-    <t>Rice alt ~ bpl pop + rice_perc + wheat_perc ( as individual)</t>
-  </si>
-  <si>
-    <t>Rice alt ~ bpl pop</t>
-  </si>
-  <si>
-    <t>Wheat alt ~ bpl pop + rice_perc + wheat_perc (as individual)</t>
-  </si>
-  <si>
-    <t>Wheat alt ~ bpl pop</t>
-  </si>
-  <si>
-    <t>bpl change rate = 1</t>
-  </si>
-  <si>
-    <t>bpl change rate = 0.95</t>
+    <t>Rice alt ~ Pop + rice_moving_perc + wheat_moving_perc</t>
+  </si>
+  <si>
+    <t>Rice alt ~ bpl pop + rice_moving_perc + wheat_moving_perc</t>
+  </si>
+  <si>
+    <t>Wheat alt ~ bpl pop + rice_moving_perc + wheat_moving_perc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rice Alt ~ Pop + rice_perc + wheat_perc </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rice alt ~ bpl pop + rice_perc + wheat_perc </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wheat alt ~ pop + rice_perc + wheat_perc </t>
+  </si>
+  <si>
+    <t>Wheat alt ~ pop + rice_moving_perc + wheat_moving_perc</t>
+  </si>
+  <si>
+    <t>Wheat alt ~ bpl pop + rice_perc + wheat_perc</t>
   </si>
 </sst>
 </file>
@@ -383,10 +377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -395,7 +389,7 @@
     <col min="2" max="2" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -403,74 +397,68 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>0.79400000000000004</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+      <c r="B3">
+        <v>0.78100000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>0.62519999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>0.78220000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>0.82799999999999996</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
+      <c r="B6">
+        <v>0.63300000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0.874</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>0.871</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>0.84599999999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>0.80800000000000005</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>0.68899999999999995</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>0.59399999999999997</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>0.754</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>0.53</v>
+      <c r="B13">
+        <v>0.84099999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>